<commit_message>
#16 Create first version of Impact overview
</commit_message>
<xml_diff>
--- a/test/test-data/example-SSB-delta.xlsx
+++ b/test/test-data/example-SSB-delta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares.sharepoint.com/teams/dlt42161/Shared Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\6svk\test\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="541" documentId="8_{59D5BCFB-ED04-4404-9339-7C8BEA929DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21135B78-F212-4C9E-820B-F8F03CE25AE9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DBB115-02BE-417D-A052-3A6B3048F71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{479C864B-AE26-47F0-AFFE-7BF700634394}"/>
+    <workbookView xWindow="-23148" yWindow="3636" windowWidth="23256" windowHeight="13896" xr2:uid="{479C864B-AE26-47F0-AFFE-7BF700634394}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="2" r:id="rId1"/>
@@ -279,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="162">
   <si>
     <t>Code van de kennisvraag bv RP_ET1</t>
   </si>
@@ -1386,9 +1386,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>48</xdr:col>
-      <xdr:colOff>393880</xdr:colOff>
+      <xdr:colOff>391975</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>203396</xdr:rowOff>
+      <xdr:rowOff>201491</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1867,9 +1867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00BDDAB-9767-41F7-8824-A78ED8C137BD}">
   <dimension ref="A1:AF82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="V31" s="14"/>
     </row>
-    <row r="32" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>80</v>
       </c>
@@ -3135,7 +3135,7 @@
       </c>
       <c r="V32" s="14"/>
     </row>
-    <row r="33" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>80</v>
       </c>
@@ -3330,7 +3330,7 @@
       </c>
       <c r="V39" s="14"/>
     </row>
-    <row r="40" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>80</v>
       </c>
@@ -3359,7 +3359,7 @@
       </c>
       <c r="V40" s="14"/>
     </row>
-    <row r="41" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>80</v>
       </c>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="V47" s="14"/>
     </row>
-    <row r="48" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>80</v>
       </c>
@@ -3783,7 +3783,7 @@
       </c>
       <c r="V55" s="14"/>
     </row>
-    <row r="56" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>80</v>
       </c>
@@ -3806,7 +3806,7 @@
       <c r="R56" s="14"/>
       <c r="V56" s="14"/>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>80</v>
       </c>
@@ -3829,7 +3829,13 @@
       <c r="R57" s="14"/>
       <c r="V57" s="14"/>
     </row>
-    <row r="58" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="6">
+        <v>56</v>
+      </c>
       <c r="D58" s="19"/>
       <c r="F58" s="13" t="s">
         <v>154</v>
@@ -3975,6 +3981,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010051F94B6AE6ED7E4A87B975BD711A42C8" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="52b9f7658f312bac273cc14b8d12ad72">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="67a1054d-5936-46ee-9c1d-1714ddbd2c93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f04d8645f5f77883ee3eff4b5c253a6" ns2:_="">
     <xsd:import namespace="67a1054d-5936-46ee-9c1d-1714ddbd2c93"/>
@@ -4112,12 +4124,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFA59E53-0119-4740-8271-E9D7B077C030}">
   <ds:schemaRefs>
@@ -4127,6 +4133,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{187EA8E7-9F49-4211-BB08-ED8EF39DD0B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="67a1054d-5936-46ee-9c1d-1714ddbd2c93"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7B3B2DB-1919-44FE-9B57-40FDC14B999E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4144,22 +4166,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{187EA8E7-9F49-4211-BB08-ED8EF39DD0B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="67a1054d-5936-46ee-9c1d-1714ddbd2c93"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{15f3fe0e-d712-4981-bc7c-fe949af215bb}" enabled="0" method="" siteId="{15f3fe0e-d712-4981-bc7c-fe949af215bb}" removed="1"/>

</xml_diff>